<commit_message>
Fixed seeding error. Made vaccine run script.
</commit_message>
<xml_diff>
--- a/PopData.xlsx
+++ b/PopData.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\Model\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Targets" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -961,19 +961,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -994,7 +985,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1032,7 +1032,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2899,7 +2898,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3836,7 +3834,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4525,7 +4522,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4648,7 +4644,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5163,7 +5158,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13275,41 +13269,41 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AP69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" customWidth="1"/>
-    <col min="8" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="16" max="16" width="17.7265625" customWidth="1"/>
-    <col min="17" max="17" width="19.90625" customWidth="1"/>
-    <col min="18" max="18" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.90625" customWidth="1"/>
-    <col min="21" max="21" width="15.453125" customWidth="1"/>
-    <col min="22" max="22" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.1796875" customWidth="1"/>
-    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.26953125" customWidth="1"/>
-    <col min="28" max="29" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.90625" customWidth="1"/>
-    <col min="31" max="31" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.1796875" customWidth="1"/>
-    <col min="33" max="33" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.90625" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" customWidth="1"/>
+    <col min="28" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" customWidth="1"/>
+    <col min="31" max="31" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:42" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -13319,35 +13313,35 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73" t="s">
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="O1" s="74" t="s">
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="O1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="P1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="77"/>
       <c r="Y1" s="3" t="s">
         <v>8</v>
       </c>
@@ -13383,7 +13377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="62" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:42" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -13393,7 +13387,7 @@
       <c r="C2" s="23">
         <v>417311</v>
       </c>
-      <c r="F2" s="72"/>
+      <c r="F2" s="69"/>
       <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
@@ -13412,16 +13406,16 @@
       <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="75"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="70" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="70" t="s">
+      <c r="S2" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="70" t="s">
+      <c r="T2" s="66" t="s">
         <v>43</v>
       </c>
       <c r="U2" s="8" t="s">
@@ -13456,16 +13450,16 @@
         <v>0</v>
       </c>
       <c r="AI2" s="23">
-        <f>52*5</f>
-        <v>260</v>
+        <f>52*4.5</f>
+        <v>234</v>
       </c>
       <c r="AJ2" s="23">
         <f>AI2/2</f>
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="AK2" s="23">
         <f>AI2/2.4</f>
-        <v>108.33333333333334</v>
+        <v>97.5</v>
       </c>
       <c r="AM2" t="s">
         <v>21</v>
@@ -13480,7 +13474,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="33.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:42" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -13512,12 +13506,12 @@
         <f>1-J3-K3</f>
         <v>0</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
       <c r="U3" s="10" t="s">
         <v>23</v>
       </c>
@@ -13556,16 +13550,16 @@
         <v>1</v>
       </c>
       <c r="AI3" s="23">
-        <f>52*5</f>
-        <v>260</v>
+        <f>52*4.5</f>
+        <v>234</v>
       </c>
       <c r="AJ3" s="23">
         <f>AI3/2</f>
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="AK3" s="23">
         <f>AI3/2.4</f>
-        <v>108.33333333333334</v>
+        <v>97.5</v>
       </c>
       <c r="AN3" s="25">
         <v>1988</v>
@@ -13577,7 +13571,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -13679,7 +13673,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -13761,7 +13755,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -13844,7 +13838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -13924,7 +13918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -14006,13 +14000,13 @@
       <c r="AG8" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="AJ8" s="66" t="s">
+      <c r="AJ8" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="AK8" s="66"/>
-      <c r="AL8" s="66"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="74"/>
     </row>
-    <row r="9" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -14107,7 +14101,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>35</v>
       </c>
@@ -14199,7 +14193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
@@ -14291,7 +14285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>37</v>
       </c>
@@ -14381,18 +14375,18 @@
       </c>
       <c r="AJ12" s="42">
         <f>AI2*$AI$12</f>
-        <v>65</v>
+        <v>58.5</v>
       </c>
       <c r="AK12" s="42">
         <f>AJ2*$AI$12</f>
-        <v>32.5</v>
+        <v>29.25</v>
       </c>
       <c r="AL12" s="42">
         <f>AK2*$AI$12</f>
-        <v>27.083333333333336</v>
+        <v>24.375</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="55" t="s">
         <v>38</v>
       </c>
@@ -14482,18 +14476,18 @@
       </c>
       <c r="AJ13" s="42">
         <f>AJ14*$AI$13</f>
-        <v>254.79999999999998</v>
+        <v>229.32</v>
       </c>
       <c r="AK13" s="42">
         <f>AK14*$AI$13</f>
-        <v>127.39999999999999</v>
+        <v>114.66</v>
       </c>
       <c r="AL13" s="42">
         <f>AL14*$AI$13</f>
-        <v>106.16666666666667</v>
+        <v>95.55</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
         <v>97</v>
       </c>
@@ -14586,18 +14580,18 @@
       </c>
       <c r="AJ14" s="42">
         <f>AI2</f>
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="AK14" s="42">
         <f>AJ2</f>
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="AL14" s="42">
         <f>AK2</f>
-        <v>108.33333333333334</v>
+        <v>97.5</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
         <v>98</v>
       </c>
@@ -14690,18 +14684,18 @@
       </c>
       <c r="AJ15" s="42">
         <f t="shared" ref="AJ15:AJ25" si="3">$AJ$14*AI15</f>
-        <v>218.63306796596578</v>
+        <v>196.76976116936919</v>
       </c>
       <c r="AK15" s="42">
         <f t="shared" ref="AK15:AK25" si="4">$AK$14*AI15</f>
-        <v>109.31653398298289</v>
+        <v>98.384880584684595</v>
       </c>
       <c r="AL15" s="42">
         <f t="shared" ref="AL15:AL25" si="5">$AL$14*AI15</f>
-        <v>91.097111652485751</v>
+        <v>81.987400487237167</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
         <v>99</v>
       </c>
@@ -14794,18 +14788,18 @@
       </c>
       <c r="AJ16" s="42">
         <f t="shared" si="3"/>
-        <v>183.84776310850236</v>
+        <v>165.46298679765212</v>
       </c>
       <c r="AK16" s="42">
         <f t="shared" si="4"/>
-        <v>91.923881554251182</v>
+        <v>82.731493398826061</v>
       </c>
       <c r="AL16" s="42">
         <f t="shared" si="5"/>
-        <v>76.603234628542666</v>
+        <v>68.942911165688386</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="53" t="s">
         <v>100</v>
       </c>
@@ -14898,18 +14892,18 @@
       </c>
       <c r="AJ17" s="42">
         <f t="shared" si="3"/>
-        <v>154.59692495035372</v>
+        <v>139.13723245531835</v>
       </c>
       <c r="AK17" s="42">
         <f t="shared" si="4"/>
-        <v>77.298462475176862</v>
+        <v>69.568616227659177</v>
       </c>
       <c r="AL17" s="42">
         <f t="shared" si="5"/>
-        <v>64.415385395980735</v>
+        <v>57.97384685638265</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58" t="s">
         <v>44</v>
       </c>
@@ -15007,18 +15001,18 @@
       </c>
       <c r="AJ18" s="42">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="AK18" s="42">
         <f t="shared" si="4"/>
-        <v>65</v>
+        <v>58.5</v>
       </c>
       <c r="AL18" s="42">
         <f t="shared" si="5"/>
-        <v>54.166666666666671</v>
+        <v>48.75</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="O19" s="53" t="s">
@@ -15060,18 +15054,18 @@
       </c>
       <c r="AJ19" s="42">
         <f t="shared" si="3"/>
-        <v>109.31653398298289</v>
+        <v>98.384880584684595</v>
       </c>
       <c r="AK19" s="42">
         <f t="shared" si="4"/>
-        <v>54.658266991491445</v>
+        <v>49.192440292342297</v>
       </c>
       <c r="AL19" s="42">
         <f t="shared" si="5"/>
-        <v>45.548555826242875</v>
+        <v>40.993700243618584</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="AG20" s="48" t="s">
@@ -15086,18 +15080,18 @@
       </c>
       <c r="AJ20" s="42">
         <f t="shared" si="3"/>
-        <v>91.923881554251182</v>
+        <v>82.731493398826061</v>
       </c>
       <c r="AK20" s="42">
         <f t="shared" si="4"/>
-        <v>45.961940777125591</v>
+        <v>41.36574669941303</v>
       </c>
       <c r="AL20" s="42">
         <f t="shared" si="5"/>
-        <v>38.301617314271333</v>
+        <v>34.471455582844193</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="Y21" t="s">
         <v>84</v>
       </c>
@@ -15113,18 +15107,18 @@
       </c>
       <c r="AJ21" s="42">
         <f t="shared" si="3"/>
-        <v>77.298462475176876</v>
+        <v>69.568616227659192</v>
       </c>
       <c r="AK21" s="42">
         <f t="shared" si="4"/>
-        <v>38.649231237588438</v>
+        <v>34.784308113829596</v>
       </c>
       <c r="AL21" s="42">
         <f t="shared" si="5"/>
-        <v>32.207692697990367</v>
+        <v>28.986923428191332</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="Y22" s="13" t="s">
@@ -15142,18 +15136,18 @@
       </c>
       <c r="AJ22" s="42">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>58.5</v>
       </c>
       <c r="AK22" s="42">
         <f t="shared" si="4"/>
-        <v>32.5</v>
+        <v>29.25</v>
       </c>
       <c r="AL22" s="42">
         <f t="shared" si="5"/>
-        <v>27.083333333333336</v>
+        <v>24.375</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>39</v>
       </c>
@@ -15189,18 +15183,18 @@
       </c>
       <c r="AJ23" s="42">
         <f t="shared" si="3"/>
-        <v>54.658266991491452</v>
+        <v>49.192440292342305</v>
       </c>
       <c r="AK23" s="42">
         <f t="shared" si="4"/>
-        <v>27.329133495745726</v>
+        <v>24.596220146171152</v>
       </c>
       <c r="AL23" s="42">
         <f t="shared" si="5"/>
-        <v>22.774277913121438</v>
+        <v>20.496850121809295</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="O24" s="40" t="s">
@@ -15238,18 +15232,18 @@
       </c>
       <c r="AJ24" s="42">
         <f t="shared" si="3"/>
-        <v>45.961940777125591</v>
+        <v>41.36574669941303</v>
       </c>
       <c r="AK24" s="42">
         <f t="shared" si="4"/>
-        <v>22.980970388562795</v>
+        <v>20.682873349706515</v>
       </c>
       <c r="AL24" s="42">
         <f t="shared" si="5"/>
-        <v>19.150808657135666</v>
+        <v>17.235727791422097</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AG25" s="48" t="s">
         <v>100</v>
       </c>
@@ -15262,41 +15256,41 @@
       </c>
       <c r="AJ25" s="42">
         <f t="shared" si="3"/>
-        <v>38.649231237588438</v>
+        <v>34.784308113829596</v>
       </c>
       <c r="AK25" s="42">
         <f t="shared" si="4"/>
-        <v>19.324615618794219</v>
+        <v>17.392154056914798</v>
       </c>
       <c r="AL25" s="42">
         <f t="shared" si="5"/>
-        <v>16.103846348995184</v>
+        <v>14.493461714095666</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L26" s="14"/>
       <c r="AI26" s="50"/>
       <c r="AJ26" s="51"/>
       <c r="AK26" s="51"/>
       <c r="AL26" s="51"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AI27" s="50"/>
       <c r="AJ27" s="51"/>
       <c r="AK27" s="51"/>
       <c r="AL27" s="51"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AG30" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="AJ30" s="66" t="s">
+      <c r="AJ30" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="AK30" s="66"/>
-      <c r="AL30" s="66"/>
+      <c r="AK30" s="74"/>
+      <c r="AL30" s="74"/>
     </row>
-    <row r="31" spans="1:38" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="59" t="s">
         <v>107</v>
       </c>
@@ -15342,7 +15336,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="O32" s="32"/>
       <c r="P32" s="32"/>
       <c r="Q32" s="32"/>
@@ -15373,7 +15367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="O33" s="33"/>
       <c r="P33" s="34">
         <v>1990</v>
@@ -15436,7 +15430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="O34" s="35" t="s">
         <v>74</v>
       </c>
@@ -15496,18 +15490,18 @@
       </c>
       <c r="AJ34" s="43">
         <f>AI34*$AJ$36</f>
-        <v>70.2</v>
+        <v>63.180000000000007</v>
       </c>
       <c r="AK34" s="43">
         <f>AK36*AI34</f>
-        <v>35.1</v>
+        <v>31.590000000000003</v>
       </c>
       <c r="AL34" s="43">
         <f>AL36*AI34</f>
-        <v>29.250000000000004</v>
+        <v>26.325000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -15576,18 +15570,18 @@
       </c>
       <c r="AJ35" s="43">
         <f>AI35*$AJ$36</f>
-        <v>234</v>
+        <v>210.6</v>
       </c>
       <c r="AK35" s="43">
         <f>AI35*AK36</f>
-        <v>117</v>
+        <v>105.3</v>
       </c>
       <c r="AL35" s="43">
         <f>AL36*AI35</f>
-        <v>97.500000000000014</v>
+        <v>87.75</v>
       </c>
     </row>
-    <row r="36" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>15</v>
       </c>
@@ -15661,18 +15655,18 @@
       </c>
       <c r="AJ36" s="43">
         <f>AI3</f>
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="AK36" s="43">
         <f>AJ3</f>
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="AL36" s="43">
         <f>AK3</f>
-        <v>108.33333333333334</v>
+        <v>97.5</v>
       </c>
     </row>
-    <row r="37" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
@@ -15745,18 +15739,18 @@
       </c>
       <c r="AJ37" s="43">
         <f t="shared" ref="AJ37:AJ47" si="7">$AJ$36*AI37</f>
-        <v>218.63306796596578</v>
+        <v>196.76976116936919</v>
       </c>
       <c r="AK37" s="43">
         <f t="shared" ref="AK37:AK47" si="8">$AK$36*AI37</f>
-        <v>109.31653398298289</v>
+        <v>98.384880584684595</v>
       </c>
       <c r="AL37" s="43">
         <f>$AK$3*AI37</f>
-        <v>91.097111652485751</v>
+        <v>81.987400487237167</v>
       </c>
     </row>
-    <row r="38" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>25</v>
       </c>
@@ -15829,18 +15823,18 @@
       </c>
       <c r="AJ38" s="43">
         <f t="shared" si="7"/>
-        <v>183.84776310850236</v>
+        <v>165.46298679765212</v>
       </c>
       <c r="AK38" s="43">
         <f t="shared" si="8"/>
-        <v>91.923881554251182</v>
+        <v>82.731493398826061</v>
       </c>
       <c r="AL38" s="43">
         <f t="shared" ref="AL38:AL43" si="9">$AK$3*AI38</f>
-        <v>76.603234628542666</v>
+        <v>68.942911165688386</v>
       </c>
     </row>
-    <row r="39" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>28</v>
       </c>
@@ -15913,18 +15907,18 @@
       </c>
       <c r="AJ39" s="43">
         <f t="shared" si="7"/>
-        <v>154.59692495035372</v>
+        <v>139.13723245531835</v>
       </c>
       <c r="AK39" s="43">
         <f t="shared" si="8"/>
-        <v>77.298462475176862</v>
+        <v>69.568616227659177</v>
       </c>
       <c r="AL39" s="43">
         <f t="shared" si="9"/>
-        <v>64.415385395980735</v>
+        <v>57.97384685638265</v>
       </c>
     </row>
-    <row r="40" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>30</v>
       </c>
@@ -15997,18 +15991,18 @@
       </c>
       <c r="AJ40" s="43">
         <f t="shared" si="7"/>
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="AK40" s="43">
         <f t="shared" si="8"/>
-        <v>65</v>
+        <v>58.5</v>
       </c>
       <c r="AL40" s="43">
         <f t="shared" si="9"/>
-        <v>54.166666666666671</v>
+        <v>48.75</v>
       </c>
     </row>
-    <row r="41" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>31</v>
       </c>
@@ -16081,18 +16075,18 @@
       </c>
       <c r="AJ41" s="43">
         <f t="shared" si="7"/>
-        <v>109.31653398298289</v>
+        <v>98.384880584684595</v>
       </c>
       <c r="AK41" s="43">
         <f t="shared" si="8"/>
-        <v>54.658266991491445</v>
+        <v>49.192440292342297</v>
       </c>
       <c r="AL41" s="43">
         <f t="shared" si="9"/>
-        <v>45.548555826242875</v>
+        <v>40.993700243618584</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
@@ -16165,18 +16159,18 @@
       </c>
       <c r="AJ42" s="43">
         <f t="shared" si="7"/>
-        <v>91.923881554251182</v>
+        <v>82.731493398826061</v>
       </c>
       <c r="AK42" s="43">
         <f t="shared" si="8"/>
-        <v>45.961940777125591</v>
+        <v>41.36574669941303</v>
       </c>
       <c r="AL42" s="43">
         <f t="shared" si="9"/>
-        <v>38.301617314271333</v>
+        <v>34.471455582844193</v>
       </c>
     </row>
-    <row r="43" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>33</v>
       </c>
@@ -16249,18 +16243,18 @@
       </c>
       <c r="AJ43" s="43">
         <f t="shared" si="7"/>
-        <v>77.298462475176876</v>
+        <v>69.568616227659192</v>
       </c>
       <c r="AK43" s="43">
         <f t="shared" si="8"/>
-        <v>38.649231237588438</v>
+        <v>34.784308113829596</v>
       </c>
       <c r="AL43" s="43">
         <f t="shared" si="9"/>
-        <v>32.207692697990367</v>
+        <v>28.986923428191332</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>35</v>
       </c>
@@ -16333,18 +16327,18 @@
       </c>
       <c r="AJ44" s="43">
         <f t="shared" si="7"/>
-        <v>65</v>
+        <v>58.5</v>
       </c>
       <c r="AK44" s="43">
         <f t="shared" si="8"/>
-        <v>32.5</v>
+        <v>29.25</v>
       </c>
       <c r="AL44" s="43">
         <f t="shared" ref="AL44:AL47" si="11">$AK$3*AI44</f>
-        <v>27.083333333333336</v>
+        <v>24.375</v>
       </c>
     </row>
-    <row r="45" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
@@ -16417,18 +16411,18 @@
       </c>
       <c r="AJ45" s="43">
         <f t="shared" si="7"/>
-        <v>54.658266991491452</v>
+        <v>49.192440292342305</v>
       </c>
       <c r="AK45" s="43">
         <f t="shared" si="8"/>
-        <v>27.329133495745726</v>
+        <v>24.596220146171152</v>
       </c>
       <c r="AL45" s="43">
         <f t="shared" si="11"/>
-        <v>22.774277913121438</v>
+        <v>20.496850121809295</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>37</v>
       </c>
@@ -16501,18 +16495,18 @@
       </c>
       <c r="AJ46" s="43">
         <f t="shared" si="7"/>
-        <v>45.961940777125591</v>
+        <v>41.36574669941303</v>
       </c>
       <c r="AK46" s="43">
         <f t="shared" si="8"/>
-        <v>22.980970388562795</v>
+        <v>20.682873349706515</v>
       </c>
       <c r="AL46" s="43">
         <f t="shared" si="11"/>
-        <v>19.150808657135666</v>
+        <v>17.235727791422097</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="55" t="s">
         <v>38</v>
       </c>
@@ -16545,18 +16539,18 @@
       </c>
       <c r="AJ47" s="43">
         <f t="shared" si="7"/>
-        <v>38.649231237588438</v>
+        <v>34.784308113829596</v>
       </c>
       <c r="AK47" s="43">
         <f t="shared" si="8"/>
-        <v>19.324615618794219</v>
+        <v>17.392154056914798</v>
       </c>
       <c r="AL47" s="43">
         <f t="shared" si="11"/>
-        <v>16.103846348995184</v>
+        <v>14.493461714095666</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:38" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A48" s="53" t="s">
         <v>97</v>
       </c>
@@ -16571,7 +16565,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
         <v>98</v>
       </c>
@@ -16583,7 +16577,7 @@
         <v>44482.861635220121</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="53" t="s">
         <v>99</v>
       </c>
@@ -16598,7 +16592,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="53" t="s">
         <v>100</v>
       </c>
@@ -16610,15 +16604,15 @@
         <v>22783.176100628931</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O53" s="29"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O62" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O63" t="s">
         <v>68</v>
       </c>
@@ -16626,7 +16620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O64" t="s">
         <v>0</v>
       </c>
@@ -16637,7 +16631,7 @@
         <v>0.23480000000000001</v>
       </c>
     </row>
-    <row r="65" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="15:17" x14ac:dyDescent="0.25">
       <c r="O65" t="s">
         <v>1</v>
       </c>
@@ -16648,7 +16642,7 @@
         <v>0.21460000000000001</v>
       </c>
     </row>
-    <row r="69" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="15:17" x14ac:dyDescent="0.25">
       <c r="O69">
         <f>NORMDIST(0.7, P64,Q64,TRUE)</f>
         <v>0.78945004503905036</v>
@@ -16656,18 +16650,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AJ8:AL8"/>
+    <mergeCell ref="AJ30:AL30"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="O1:O3"/>
     <mergeCell ref="P1:P3"/>
-    <mergeCell ref="AJ8:AL8"/>
-    <mergeCell ref="AJ30:AL30"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16684,23 +16678,22 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="12" max="12" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="10.26953125" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" customWidth="1"/>
-    <col min="16" max="16" width="11.36328125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="15" max="16" width="11.42578125" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T2" t="s">
         <v>54</v>
       </c>
@@ -16708,7 +16701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="78">
         <v>1996</v>
@@ -16750,7 +16743,7 @@
         <v>5420315</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -16810,7 +16803,7 @@
         <v>8068284</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>45</v>
       </c>
@@ -16870,7 +16863,7 @@
         <v>9138179</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>46</v>
       </c>
@@ -16930,7 +16923,7 @@
         <v>10267300</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>47</v>
       </c>
@@ -16990,7 +16983,7 @@
         <v>10456909</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -17037,7 +17030,7 @@
         <v>10571313</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S9" t="s">
         <v>70</v>
       </c>
@@ -17048,7 +17041,7 @@
         <v>10688168</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>51</v>
       </c>
@@ -17102,7 +17095,7 @@
         <v>10806536</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S11" t="s">
         <v>70</v>
       </c>
@@ -17113,7 +17106,7 @@
         <v>10924776</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -17127,7 +17120,7 @@
         <v>11039740</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>50</v>
       </c>
@@ -17141,7 +17134,7 @@
         <v>11155657</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>52</v>
       </c>
@@ -17150,7 +17143,7 @@
         <v>5.1649773565416463E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -17159,12 +17152,12 @@
         <v>2.0659909426166585E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>54</v>
       </c>
@@ -17172,7 +17165,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>1990</v>
       </c>
@@ -17186,7 +17179,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>1991</v>
       </c>
@@ -17194,7 +17187,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>1992</v>
       </c>
@@ -17202,7 +17195,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>1993</v>
       </c>
@@ -17210,7 +17203,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>1994</v>
       </c>
@@ -17218,7 +17211,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>1995</v>
       </c>
@@ -17226,7 +17219,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>1996</v>
       </c>
@@ -17234,7 +17227,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>1997</v>
       </c>
@@ -17242,7 +17235,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>1998</v>
       </c>
@@ -17250,7 +17243,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>1999</v>
       </c>
@@ -17258,7 +17251,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>2000</v>
       </c>
@@ -17266,7 +17259,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>2001</v>
       </c>
@@ -17280,7 +17273,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>2002</v>
       </c>
@@ -17288,7 +17281,7 @@
         <v>0.24299999999999999</v>
       </c>
     </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>2003</v>
       </c>
@@ -17296,7 +17289,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>2004</v>
       </c>
@@ -17304,7 +17297,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>2005</v>
       </c>
@@ -17312,7 +17305,7 @@
         <v>0.26100000000000001</v>
       </c>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E49">
         <v>2006</v>
       </c>
@@ -17320,7 +17313,7 @@
         <v>0.26100000000000001</v>
       </c>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E50">
         <v>2007</v>
       </c>
@@ -17328,7 +17321,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E51">
         <v>2008</v>
       </c>
@@ -17336,7 +17329,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E52">
         <v>2009</v>
       </c>
@@ -17344,7 +17337,7 @@
         <v>0.26300000000000001</v>
       </c>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E53">
         <v>2010</v>
       </c>
@@ -17352,7 +17345,7 @@
         <v>0.26300000000000001</v>
       </c>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E54">
         <v>2012</v>
       </c>
@@ -17363,7 +17356,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F55" s="26"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ported over changes from CSDE cluster
</commit_message>
<xml_diff>
--- a/PopData.xlsx
+++ b/PopData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -517,7 +517,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,9 +597,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -628,7 +646,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -804,11 +822,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -911,8 +940,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -924,10 +951,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -961,13 +984,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -985,21 +1017,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3834,6 +3871,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4522,6 +4560,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13269,41 +13308,41 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AP69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="8" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="8" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" customWidth="1"/>
-    <col min="28" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.140625" customWidth="1"/>
-    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" customWidth="1"/>
+    <col min="17" max="17" width="19.81640625" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.81640625" customWidth="1"/>
+    <col min="21" max="21" width="15.453125" customWidth="1"/>
+    <col min="22" max="22" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1796875" customWidth="1"/>
+    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.26953125" customWidth="1"/>
+    <col min="28" max="29" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.81640625" customWidth="1"/>
+    <col min="31" max="31" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.1796875" customWidth="1"/>
+    <col min="33" max="33" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -13313,35 +13352,35 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70" t="s">
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="O1" s="71" t="s">
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="O1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="P1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="75" t="s">
+      <c r="R1" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="77"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="62"/>
       <c r="Y1" s="3" t="s">
         <v>8</v>
       </c>
@@ -13377,7 +13416,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" ht="62" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -13387,7 +13426,7 @@
       <c r="C2" s="23">
         <v>417311</v>
       </c>
-      <c r="F2" s="69"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
@@ -13406,16 +13445,16 @@
       <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="66" t="s">
+      <c r="O2" s="69"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="66" t="s">
+      <c r="S2" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="66" t="s">
+      <c r="T2" s="63" t="s">
         <v>43</v>
       </c>
       <c r="U2" s="8" t="s">
@@ -13443,23 +13482,23 @@
       <c r="AD2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="45" t="s">
+      <c r="AE2" s="43" t="s">
         <v>11</v>
       </c>
       <c r="AH2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="AI2" s="23">
+      <c r="AI2" s="73">
         <f>52*4.5</f>
         <v>234</v>
       </c>
-      <c r="AJ2" s="23">
-        <f>AI2/2</f>
-        <v>117</v>
-      </c>
-      <c r="AK2" s="23">
-        <f>AI2/2.4</f>
-        <v>97.5</v>
+      <c r="AJ2" s="73">
+        <f>AI2*0.6</f>
+        <v>140.4</v>
+      </c>
+      <c r="AK2" s="73">
+        <f>AJ2*0.6</f>
+        <v>84.24</v>
       </c>
       <c r="AM2" t="s">
         <v>21</v>
@@ -13467,14 +13506,14 @@
       <c r="AN2" s="25">
         <v>1985</v>
       </c>
-      <c r="AO2" s="23">
-        <v>0.2</v>
-      </c>
-      <c r="AP2" s="23">
-        <v>0.2</v>
+      <c r="AO2" s="73">
+        <v>0.3</v>
+      </c>
+      <c r="AP2" s="73">
+        <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -13506,12 +13545,12 @@
         <f>1-J3-K3</f>
         <v>0</v>
       </c>
-      <c r="O3" s="73"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
       <c r="U3" s="10" t="s">
         <v>23</v>
       </c>
@@ -13549,29 +13588,29 @@
       <c r="AH3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AI3" s="23">
+      <c r="AI3" s="73">
         <f>52*4.5</f>
         <v>234</v>
       </c>
-      <c r="AJ3" s="23">
-        <f>AI3/2</f>
-        <v>117</v>
-      </c>
-      <c r="AK3" s="23">
-        <f>AI3/2.4</f>
-        <v>97.5</v>
+      <c r="AJ3" s="73">
+        <f>AI3*0.6</f>
+        <v>140.4</v>
+      </c>
+      <c r="AK3" s="73">
+        <f>AJ3*0.6</f>
+        <v>84.24</v>
       </c>
       <c r="AN3" s="25">
         <v>1988</v>
       </c>
-      <c r="AO3" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="AP3" s="23">
-        <v>0.3</v>
+      <c r="AO3" s="73">
+        <v>0.4</v>
+      </c>
+      <c r="AP3" s="73">
+        <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -13666,14 +13705,14 @@
       <c r="AN4" s="25">
         <v>2003</v>
       </c>
-      <c r="AO4" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="AP4" s="23">
-        <v>0.1</v>
+      <c r="AO4" s="73">
+        <v>0.3</v>
+      </c>
+      <c r="AP4" s="73">
+        <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -13748,14 +13787,14 @@
       <c r="AC5" s="23">
         <v>1.2E-2</v>
       </c>
-      <c r="AD5" s="44">
+      <c r="AD5" s="42">
         <v>0.12</v>
       </c>
-      <c r="AE5" s="46">
+      <c r="AE5" s="44">
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -13828,17 +13867,17 @@
       <c r="AC6" s="23">
         <v>0.66959798994974873</v>
       </c>
-      <c r="AD6" s="44">
+      <c r="AD6" s="42">
         <v>2.2142857142857144</v>
       </c>
-      <c r="AE6" s="47">
+      <c r="AE6" s="45">
         <v>6.5</v>
       </c>
       <c r="AN6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -13911,14 +13950,14 @@
       <c r="AC7" s="23">
         <v>0.79487179487179482</v>
       </c>
-      <c r="AD7" s="44">
+      <c r="AD7" s="42">
         <v>2.25</v>
       </c>
-      <c r="AE7" s="47">
+      <c r="AE7" s="45">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -13991,22 +14030,24 @@
       <c r="AC8" s="23">
         <v>0.80509304603330067</v>
       </c>
-      <c r="AD8" s="44">
+      <c r="AD8" s="42">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE8" s="47">
+      <c r="AE8" s="45">
         <v>5.333333333333333</v>
       </c>
-      <c r="AG8" s="18" t="s">
+      <c r="AG8" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="AJ8" s="74" t="s">
+      <c r="AH8" s="72"/>
+      <c r="AI8" s="72"/>
+      <c r="AJ8" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="AK8" s="74"/>
-      <c r="AL8" s="74"/>
+      <c r="AK8" s="75"/>
+      <c r="AL8" s="75"/>
     </row>
-    <row r="9" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -14079,29 +14120,30 @@
       <c r="AC9" s="23">
         <v>0.75512405609492983</v>
       </c>
-      <c r="AD9" s="44">
+      <c r="AD9" s="42">
         <v>2.0625</v>
       </c>
-      <c r="AE9" s="47">
+      <c r="AE9" s="45">
         <v>0</v>
       </c>
-      <c r="AG9" s="18" t="s">
+      <c r="AG9" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="AI9" s="18" t="s">
+      <c r="AH9" s="72"/>
+      <c r="AI9" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="AJ9" s="18" t="s">
+      <c r="AJ9" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="AK9" s="52" t="s">
+      <c r="AK9" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="AL9" s="18" t="s">
+      <c r="AL9" s="74" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>35</v>
       </c>
@@ -14174,26 +14216,28 @@
       <c r="AC10" s="23">
         <v>0.75529411764705878</v>
       </c>
-      <c r="AD10" s="44">
+      <c r="AD10" s="42">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE10" s="47">
+      <c r="AE10" s="45">
         <v>9</v>
       </c>
-      <c r="AG10" s="48" t="s">
+      <c r="AG10" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="AJ10" s="43">
+      <c r="AH10" s="72"/>
+      <c r="AI10" s="72"/>
+      <c r="AJ10" s="77">
         <v>0</v>
       </c>
-      <c r="AK10" s="43">
+      <c r="AK10" s="77">
         <v>0</v>
       </c>
-      <c r="AL10" s="43">
+      <c r="AL10" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
@@ -14266,26 +14310,28 @@
       <c r="AC11" s="23">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD11" s="44">
+      <c r="AD11" s="42">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE11" s="47">
+      <c r="AE11" s="45">
         <v>0</v>
       </c>
-      <c r="AG11" s="48" t="s">
+      <c r="AG11" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="AJ11" s="43">
+      <c r="AH11" s="72"/>
+      <c r="AI11" s="72"/>
+      <c r="AJ11" s="77">
         <v>0</v>
       </c>
-      <c r="AK11" s="43">
+      <c r="AK11" s="77">
         <v>0</v>
       </c>
-      <c r="AL11" s="43">
+      <c r="AL11" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>37</v>
       </c>
@@ -14358,42 +14404,37 @@
       <c r="AC12" s="23">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD12" s="44">
+      <c r="AD12" s="42">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE12" s="47">
+      <c r="AE12" s="45">
         <v>0</v>
       </c>
-      <c r="AG12" s="48" t="s">
+      <c r="AG12" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="AH12" s="12">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AJ12" s="42">
-        <f>AI2*$AI$12</f>
-        <v>58.5</v>
-      </c>
-      <c r="AK12" s="42">
-        <f>AJ2*$AI$12</f>
-        <v>29.25</v>
-      </c>
-      <c r="AL12" s="42">
-        <f>AK2*$AI$12</f>
-        <v>24.375</v>
+      <c r="AH12" s="72"/>
+      <c r="AI12" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="AJ12" s="79">
+        <v>11.700000000000001</v>
+      </c>
+      <c r="AK12" s="79">
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="AL12" s="79">
+        <v>4.2119999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+    <row r="13" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="56">
+      <c r="B13" s="50">
         <v>70487</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="50">
         <v>82330</v>
       </c>
       <c r="F13" s="11" t="s">
@@ -14459,43 +14500,41 @@
       <c r="AC13" s="23">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD13" s="44">
+      <c r="AD13" s="42">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE13" s="47">
+      <c r="AE13" s="45">
         <v>0</v>
       </c>
-      <c r="AG13" s="48" t="s">
+      <c r="AG13" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="AH13" s="12">
-        <v>5</v>
-      </c>
-      <c r="AI13" s="12">
-        <v>0.98</v>
-      </c>
-      <c r="AJ13" s="42">
-        <f>AJ14*$AI$13</f>
-        <v>229.32</v>
-      </c>
-      <c r="AK13" s="42">
-        <f>AK14*$AI$13</f>
-        <v>114.66</v>
-      </c>
-      <c r="AL13" s="42">
-        <f>AL14*$AI$13</f>
-        <v>95.55</v>
+      <c r="AH13" s="72"/>
+      <c r="AI13" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="AJ13" s="79">
+        <f>AJ15*$AI$13</f>
+        <v>23.400000000000002</v>
+      </c>
+      <c r="AK13" s="79">
+        <f>AK15*$AI$13</f>
+        <v>14.040000000000001</v>
+      </c>
+      <c r="AL13" s="79">
+        <f>AL15*$AI$13</f>
+        <v>8.4239999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53" t="s">
+    <row r="14" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="57">
+      <c r="B14" s="51">
         <f>314094/6.27</f>
         <v>50094.736842105267</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="51">
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
@@ -14562,66 +14601,63 @@
       <c r="AC14" s="23">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD14" s="44">
+      <c r="AD14" s="42">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE14" s="47">
+      <c r="AE14" s="45">
         <v>0</v>
       </c>
-      <c r="AG14" s="48" t="s">
+      <c r="AG14" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="AH14" s="12">
-        <v>10</v>
-      </c>
-      <c r="AI14">
-        <f t="shared" ref="AI14:AI25" si="2">EXP(LN(0.5)*AH12/20)</f>
-        <v>0.9659363289248456</v>
-      </c>
-      <c r="AJ14" s="42">
-        <f>AI2</f>
-        <v>234</v>
-      </c>
-      <c r="AK14" s="42">
-        <f>AJ2</f>
-        <v>117</v>
-      </c>
-      <c r="AL14" s="42">
-        <f>AK2</f>
-        <v>97.5</v>
+      <c r="AH14" s="72"/>
+      <c r="AI14" s="72">
+        <v>0.7</v>
+      </c>
+      <c r="AJ14" s="77">
+        <f>AJ15*AI14</f>
+        <v>163.79999999999998</v>
+      </c>
+      <c r="AK14" s="77">
+        <f>AK15*AI14</f>
+        <v>98.28</v>
+      </c>
+      <c r="AL14" s="77">
+        <f>AL15*AI14</f>
+        <v>58.967999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="53" t="s">
+    <row r="15" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="57">
+      <c r="B15" s="51">
         <f>224490/6.27</f>
         <v>35803.827751196171</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="51">
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="48">
         <v>0.85074626865671632</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H15" s="48">
         <v>0.14925373134328357</v>
       </c>
-      <c r="I15" s="54">
+      <c r="I15" s="48">
         <v>0</v>
       </c>
-      <c r="J15" s="54">
+      <c r="J15" s="48">
         <v>0.99568965517241381</v>
       </c>
-      <c r="K15" s="54">
+      <c r="K15" s="48">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="L15" s="54">
+      <c r="L15" s="48">
         <v>1.4367816091954023E-3</v>
       </c>
       <c r="O15" s="6" t="s">
@@ -14651,260 +14687,254 @@
       <c r="W15" s="23">
         <v>0</v>
       </c>
-      <c r="Y15" s="53" t="s">
+      <c r="Y15" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="Z15" s="60">
+      <c r="Z15" s="54">
         <v>0.7192982456140351</v>
       </c>
-      <c r="AA15" s="60">
+      <c r="AA15" s="54">
         <v>2.3250000000000002</v>
       </c>
-      <c r="AB15" s="60">
+      <c r="AB15" s="54">
         <v>0</v>
       </c>
-      <c r="AC15" s="60">
+      <c r="AC15" s="54">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD15" s="61">
+      <c r="AD15" s="55">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE15" s="62">
+      <c r="AE15" s="56">
         <v>0</v>
       </c>
-      <c r="AG15" s="48" t="s">
+      <c r="AG15" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="AH15" s="12">
-        <v>15</v>
-      </c>
-      <c r="AI15">
-        <f t="shared" si="2"/>
-        <v>0.8408964152537145</v>
-      </c>
-      <c r="AJ15" s="42">
-        <f t="shared" ref="AJ15:AJ25" si="3">$AJ$14*AI15</f>
-        <v>196.76976116936919</v>
-      </c>
-      <c r="AK15" s="42">
-        <f t="shared" ref="AK15:AK25" si="4">$AK$14*AI15</f>
-        <v>98.384880584684595</v>
-      </c>
-      <c r="AL15" s="42">
-        <f t="shared" ref="AL15:AL25" si="5">$AL$14*AI15</f>
-        <v>81.987400487237167</v>
+      <c r="AH15" s="78">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="72"/>
+      <c r="AJ15" s="79">
+        <v>234</v>
+      </c>
+      <c r="AK15" s="79">
+        <v>140.4</v>
+      </c>
+      <c r="AL15" s="79">
+        <v>84.24</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
+    <row r="16" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="51">
         <f>151123/6.27</f>
         <v>24102.551834130783</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="51">
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="54">
+      <c r="G16" s="48">
         <v>0.85074626865671632</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="48">
         <v>0.14925373134328357</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="48">
         <v>0</v>
       </c>
-      <c r="J16" s="54">
+      <c r="J16" s="48">
         <v>0.99568965517241381</v>
       </c>
-      <c r="K16" s="54">
+      <c r="K16" s="48">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="L16" s="54">
+      <c r="L16" s="48">
         <v>1.4367816091954023E-3</v>
       </c>
-      <c r="O16" s="53" t="s">
+      <c r="O16" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="P16" s="60">
+      <c r="P16" s="54">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Q16" s="60">
+      <c r="Q16" s="54">
         <v>1.2930000000000001E-2</v>
       </c>
-      <c r="R16" s="60">
+      <c r="R16" s="54">
         <v>0</v>
       </c>
-      <c r="S16" s="60">
+      <c r="S16" s="54">
         <v>0</v>
       </c>
-      <c r="T16" s="60">
+      <c r="T16" s="54">
         <v>0</v>
       </c>
-      <c r="U16" s="60">
+      <c r="U16" s="54">
         <v>0</v>
       </c>
-      <c r="V16" s="60">
+      <c r="V16" s="54">
         <v>0</v>
       </c>
-      <c r="W16" s="60">
+      <c r="W16" s="54">
         <v>0</v>
       </c>
-      <c r="Y16" s="53" t="s">
+      <c r="Y16" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="Z16" s="60">
+      <c r="Z16" s="54">
         <v>0.7192982456140351</v>
       </c>
-      <c r="AA16" s="60">
+      <c r="AA16" s="54">
         <v>2.3250000000000002</v>
       </c>
-      <c r="AB16" s="60">
+      <c r="AB16" s="54">
         <v>0</v>
       </c>
-      <c r="AC16" s="60">
+      <c r="AC16" s="54">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD16" s="61">
+      <c r="AD16" s="55">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE16" s="62">
+      <c r="AE16" s="56">
         <v>0</v>
       </c>
-      <c r="AG16" s="48" t="s">
+      <c r="AG16" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="AH16" s="12">
-        <v>20</v>
-      </c>
-      <c r="AI16">
-        <f t="shared" si="2"/>
+      <c r="AH16" s="78">
+        <v>5</v>
+      </c>
+      <c r="AI16" s="72">
+        <f>EXP(LN(0.5)*AH16/10)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="AJ16" s="42">
-        <f t="shared" si="3"/>
+      <c r="AJ16" s="79">
+        <f>$AJ$15*AI16</f>
         <v>165.46298679765212</v>
       </c>
-      <c r="AK16" s="42">
-        <f t="shared" si="4"/>
-        <v>82.731493398826061</v>
-      </c>
-      <c r="AL16" s="42">
-        <f t="shared" si="5"/>
-        <v>68.942911165688386</v>
+      <c r="AK16" s="79">
+        <f>$AK$15*AI16</f>
+        <v>99.27779207859129</v>
+      </c>
+      <c r="AL16" s="79">
+        <f>$AL$15*AI16</f>
+        <v>59.566675247154762</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="53" t="s">
+    <row r="17" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="57">
+      <c r="B17" s="51">
         <f>89288/6.27</f>
         <v>14240.510366826158</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="51">
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="48">
         <v>0.85074626865671632</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="48">
         <v>0.14925373134328357</v>
       </c>
-      <c r="I17" s="54">
+      <c r="I17" s="48">
         <v>0</v>
       </c>
-      <c r="J17" s="54">
+      <c r="J17" s="48">
         <v>0.99568965517241381</v>
       </c>
-      <c r="K17" s="54">
+      <c r="K17" s="48">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="L17" s="54">
+      <c r="L17" s="48">
         <v>1.4367816091954023E-3</v>
       </c>
-      <c r="O17" s="53" t="s">
+      <c r="O17" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="P17" s="60">
+      <c r="P17" s="54">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Q17" s="60">
+      <c r="Q17" s="54">
         <v>1.2930000000000001E-2</v>
       </c>
-      <c r="R17" s="60">
+      <c r="R17" s="54">
         <v>0</v>
       </c>
-      <c r="S17" s="60">
+      <c r="S17" s="54">
         <v>0</v>
       </c>
-      <c r="T17" s="60">
+      <c r="T17" s="54">
         <v>0</v>
       </c>
-      <c r="U17" s="60">
+      <c r="U17" s="54">
         <v>0</v>
       </c>
-      <c r="V17" s="60">
+      <c r="V17" s="54">
         <v>0</v>
       </c>
-      <c r="W17" s="60">
+      <c r="W17" s="54">
         <v>0</v>
       </c>
-      <c r="Y17" s="53" t="s">
+      <c r="Y17" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="Z17" s="60">
+      <c r="Z17" s="54">
         <v>0.7192982456140351</v>
       </c>
-      <c r="AA17" s="60">
+      <c r="AA17" s="54">
         <v>2.3250000000000002</v>
       </c>
-      <c r="AB17" s="60">
+      <c r="AB17" s="54">
         <v>0</v>
       </c>
-      <c r="AC17" s="60">
+      <c r="AC17" s="54">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD17" s="61">
+      <c r="AD17" s="55">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE17" s="62">
+      <c r="AE17" s="56">
         <v>0</v>
       </c>
-      <c r="AG17" s="48" t="s">
+      <c r="AG17" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="AH17" s="12">
-        <v>25</v>
-      </c>
-      <c r="AI17">
-        <f t="shared" si="2"/>
-        <v>0.59460355750136051</v>
-      </c>
-      <c r="AJ17" s="42">
-        <f t="shared" si="3"/>
-        <v>139.13723245531835</v>
-      </c>
-      <c r="AK17" s="42">
-        <f t="shared" si="4"/>
-        <v>69.568616227659177</v>
-      </c>
-      <c r="AL17" s="42">
-        <f t="shared" si="5"/>
-        <v>57.97384685638265</v>
+      <c r="AH17" s="78">
+        <v>10</v>
+      </c>
+      <c r="AI17" s="72">
+        <f>EXP(LN(0.5)*AH17/10)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AJ17" s="79">
+        <f>$AJ$15*AI17</f>
+        <v>117</v>
+      </c>
+      <c r="AK17" s="79">
+        <f>$AK$15*AI17</f>
+        <v>70.2</v>
+      </c>
+      <c r="AL17" s="79">
+        <f>$AL$15*AI17</f>
+        <v>42.12</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="58" t="s">
+    <row r="18" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="52" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="20">
@@ -14919,240 +14949,240 @@
         <f>SUM(B18:C18)</f>
         <v>5703373.2934609242</v>
       </c>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="48">
         <v>0.85074626865671632</v>
       </c>
-      <c r="H18" s="54">
+      <c r="H18" s="48">
         <v>0.14925373134328357</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="48">
         <v>0</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="48">
         <v>0.99568965517241381</v>
       </c>
-      <c r="K18" s="54">
+      <c r="K18" s="48">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="L18" s="54">
+      <c r="L18" s="48">
         <v>1.4367816091954023E-3</v>
       </c>
-      <c r="O18" s="53" t="s">
+      <c r="O18" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="P18" s="60">
+      <c r="P18" s="54">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Q18" s="60">
+      <c r="Q18" s="54">
         <v>1.2930000000000001E-2</v>
       </c>
-      <c r="R18" s="60">
+      <c r="R18" s="54">
         <v>0</v>
       </c>
-      <c r="S18" s="60">
+      <c r="S18" s="54">
         <v>0</v>
       </c>
-      <c r="T18" s="60">
+      <c r="T18" s="54">
         <v>0</v>
       </c>
-      <c r="U18" s="60">
+      <c r="U18" s="54">
         <v>0</v>
       </c>
-      <c r="V18" s="60">
+      <c r="V18" s="54">
         <v>0</v>
       </c>
-      <c r="W18" s="60">
+      <c r="W18" s="54">
         <v>0</v>
       </c>
       <c r="X18" s="30"/>
-      <c r="Y18" s="53" t="s">
+      <c r="Y18" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="Z18" s="60">
+      <c r="Z18" s="54">
         <v>0.7192982456140351</v>
       </c>
-      <c r="AA18" s="60">
+      <c r="AA18" s="54">
         <v>2.3250000000000002</v>
       </c>
-      <c r="AB18" s="60">
+      <c r="AB18" s="54">
         <v>0</v>
       </c>
-      <c r="AC18" s="60">
+      <c r="AC18" s="54">
         <v>0.68708971553610498</v>
       </c>
-      <c r="AD18" s="61">
+      <c r="AD18" s="55">
         <v>2.2666666666666666</v>
       </c>
-      <c r="AE18" s="62">
+      <c r="AE18" s="56">
         <v>0</v>
       </c>
-      <c r="AG18" s="48" t="s">
+      <c r="AG18" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="AH18" s="12">
-        <v>30</v>
-      </c>
-      <c r="AI18">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="AJ18" s="42">
-        <f t="shared" si="3"/>
-        <v>117</v>
-      </c>
-      <c r="AK18" s="42">
-        <f t="shared" si="4"/>
-        <v>58.5</v>
-      </c>
-      <c r="AL18" s="42">
-        <f t="shared" si="5"/>
-        <v>48.75</v>
+      <c r="AH18" s="78">
+        <v>15</v>
+      </c>
+      <c r="AI18" s="72">
+        <f>EXP(LN(0.5)*AH18/10)</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="AJ18" s="79">
+        <f>$AJ$15*AI18</f>
+        <v>82.731493398826061</v>
+      </c>
+      <c r="AK18" s="79">
+        <f>$AK$15*AI18</f>
+        <v>49.638896039295645</v>
+      </c>
+      <c r="AL18" s="79">
+        <f>$AL$15*AI18</f>
+        <v>29.783337623577381</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="O19" s="53" t="s">
+      <c r="O19" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="P19" s="60">
+      <c r="P19" s="54">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Q19" s="60">
+      <c r="Q19" s="54">
         <v>1.2930000000000001E-2</v>
       </c>
-      <c r="R19" s="60">
+      <c r="R19" s="54">
         <v>0</v>
       </c>
-      <c r="S19" s="60">
+      <c r="S19" s="54">
         <v>0</v>
       </c>
-      <c r="T19" s="60">
+      <c r="T19" s="54">
         <v>0</v>
       </c>
-      <c r="U19" s="60">
+      <c r="U19" s="54">
         <v>0</v>
       </c>
-      <c r="V19" s="60">
+      <c r="V19" s="54">
         <v>0</v>
       </c>
-      <c r="W19" s="60">
+      <c r="W19" s="54">
         <v>0</v>
       </c>
-      <c r="AG19" s="48" t="s">
+      <c r="AG19" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="AH19" s="12">
-        <v>35</v>
-      </c>
-      <c r="AI19">
-        <f t="shared" si="2"/>
-        <v>0.42044820762685725</v>
-      </c>
-      <c r="AJ19" s="42">
-        <f t="shared" si="3"/>
-        <v>98.384880584684595</v>
-      </c>
-      <c r="AK19" s="42">
-        <f t="shared" si="4"/>
-        <v>49.192440292342297</v>
-      </c>
-      <c r="AL19" s="42">
-        <f t="shared" si="5"/>
-        <v>40.993700243618584</v>
+      <c r="AH19" s="78">
+        <v>20</v>
+      </c>
+      <c r="AI19" s="72">
+        <f>EXP(LN(0.5)*AH19/10)</f>
+        <v>0.25</v>
+      </c>
+      <c r="AJ19" s="79">
+        <f>$AJ$15*AI19</f>
+        <v>58.5</v>
+      </c>
+      <c r="AK19" s="79">
+        <f>$AK$15*AI19</f>
+        <v>35.1</v>
+      </c>
+      <c r="AL19" s="79">
+        <f>$AL$15*AI19</f>
+        <v>21.06</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="AG20" s="48" t="s">
+      <c r="AG20" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="AH20" s="12">
-        <v>40</v>
-      </c>
-      <c r="AI20">
-        <f t="shared" si="2"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="AJ20" s="42">
-        <f t="shared" si="3"/>
-        <v>82.731493398826061</v>
-      </c>
-      <c r="AK20" s="42">
-        <f t="shared" si="4"/>
+      <c r="AH20" s="78">
+        <v>25</v>
+      </c>
+      <c r="AI20" s="72">
+        <f>EXP(LN(0.5)*AH20/10)</f>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="AJ20" s="79">
+        <f>$AJ$15*AI20</f>
         <v>41.36574669941303</v>
       </c>
-      <c r="AL20" s="42">
-        <f t="shared" si="5"/>
-        <v>34.471455582844193</v>
+      <c r="AK20" s="79">
+        <f>$AK$15*AI20</f>
+        <v>24.819448019647822</v>
+      </c>
+      <c r="AL20" s="79">
+        <f>$AL$15*AI20</f>
+        <v>14.891668811788691</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="Y21" t="s">
         <v>84</v>
       </c>
-      <c r="AG21" s="48" t="s">
+      <c r="AG21" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="AH21" s="12">
-        <v>45</v>
-      </c>
-      <c r="AI21">
-        <f t="shared" si="2"/>
-        <v>0.29730177875068031</v>
-      </c>
-      <c r="AJ21" s="42">
-        <f t="shared" si="3"/>
-        <v>69.568616227659192</v>
-      </c>
-      <c r="AK21" s="42">
-        <f t="shared" si="4"/>
-        <v>34.784308113829596</v>
-      </c>
-      <c r="AL21" s="42">
-        <f t="shared" si="5"/>
-        <v>28.986923428191332</v>
+      <c r="AH21" s="78">
+        <v>30</v>
+      </c>
+      <c r="AI21" s="72">
+        <f>EXP(LN(0.5)*AH21/10)</f>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="AJ21" s="79">
+        <f>$AJ$15*AI21</f>
+        <v>29.250000000000007</v>
+      </c>
+      <c r="AK21" s="79">
+        <f>$AK$15*AI21</f>
+        <v>17.550000000000004</v>
+      </c>
+      <c r="AL21" s="79">
+        <f>$AL$15*AI21</f>
+        <v>10.530000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="Y22" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AG22" s="48" t="s">
+      <c r="AG22" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="AH22" s="12">
-        <v>50</v>
-      </c>
-      <c r="AI22">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="AJ22" s="42">
-        <f t="shared" si="3"/>
-        <v>58.5</v>
-      </c>
-      <c r="AK22" s="42">
-        <f t="shared" si="4"/>
-        <v>29.25</v>
-      </c>
-      <c r="AL22" s="42">
-        <f t="shared" si="5"/>
-        <v>24.375</v>
+      <c r="AH22" s="78">
+        <v>35</v>
+      </c>
+      <c r="AI22" s="72">
+        <f>EXP(LN(0.5)*AH22/10)</f>
+        <v>8.8388347648318447E-2</v>
+      </c>
+      <c r="AJ22" s="79">
+        <f>$AJ$15*AI22</f>
+        <v>20.682873349706515</v>
+      </c>
+      <c r="AK22" s="79">
+        <f>$AK$15*AI22</f>
+        <v>12.409724009823911</v>
+      </c>
+      <c r="AL22" s="79">
+        <f>$AL$15*AI22</f>
+        <v>7.4458344058943453</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="F23" s="48"/>
+      <c r="F23" s="46"/>
       <c r="P23" s="39" t="s">
         <v>80</v>
       </c>
@@ -15171,30 +15201,30 @@
       <c r="Y23" t="s">
         <v>29</v>
       </c>
-      <c r="AG23" s="48" t="s">
+      <c r="AG23" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="AH23" s="12">
-        <v>55</v>
-      </c>
-      <c r="AI23">
-        <f t="shared" si="2"/>
-        <v>0.21022410381342865</v>
-      </c>
-      <c r="AJ23" s="42">
-        <f t="shared" si="3"/>
-        <v>49.192440292342305</v>
-      </c>
-      <c r="AK23" s="42">
-        <f t="shared" si="4"/>
-        <v>24.596220146171152</v>
-      </c>
-      <c r="AL23" s="42">
-        <f t="shared" si="5"/>
-        <v>20.496850121809295</v>
+      <c r="AH23" s="78">
+        <v>40</v>
+      </c>
+      <c r="AI23" s="72">
+        <f>EXP(LN(0.5)*AH23/10)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AJ23" s="79">
+        <f>$AJ$15*AI23</f>
+        <v>14.625</v>
+      </c>
+      <c r="AK23" s="79">
+        <f>$AK$15*AI23</f>
+        <v>8.7750000000000004</v>
+      </c>
+      <c r="AL23" s="79">
+        <f>$AL$15*AI23</f>
+        <v>5.2649999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="30" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="O24" s="40" t="s">
@@ -15220,78 +15250,100 @@
         <f>W7/$R$7</f>
         <v>0.18971428571428572</v>
       </c>
-      <c r="AG24" s="48" t="s">
+      <c r="AG24" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="AH24" s="12">
-        <v>60</v>
-      </c>
-      <c r="AI24">
-        <f t="shared" si="2"/>
-        <v>0.17677669529663689</v>
-      </c>
-      <c r="AJ24" s="42">
-        <f t="shared" si="3"/>
-        <v>41.36574669941303</v>
-      </c>
-      <c r="AK24" s="42">
-        <f t="shared" si="4"/>
-        <v>20.682873349706515</v>
-      </c>
-      <c r="AL24" s="42">
-        <f t="shared" si="5"/>
-        <v>17.235727791422097</v>
+      <c r="AH24" s="78">
+        <v>45</v>
+      </c>
+      <c r="AI24" s="72">
+        <f>EXP(LN(0.5)*AH24/10)</f>
+        <v>4.4194173824159223E-2</v>
+      </c>
+      <c r="AJ24" s="79">
+        <f>$AJ$15*AI24</f>
+        <v>10.341436674853258</v>
+      </c>
+      <c r="AK24" s="79">
+        <f>$AK$15*AI24</f>
+        <v>6.2048620049119556</v>
+      </c>
+      <c r="AL24" s="79">
+        <f>$AL$15*AI24</f>
+        <v>3.7229172029471727</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="AG25" s="48" t="s">
+    <row r="25" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AG25" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="AH25" s="12">
-        <v>65</v>
-      </c>
-      <c r="AI25">
-        <f t="shared" si="2"/>
-        <v>0.14865088937534016</v>
-      </c>
-      <c r="AJ25" s="42">
-        <f t="shared" si="3"/>
-        <v>34.784308113829596</v>
-      </c>
-      <c r="AK25" s="42">
-        <f t="shared" si="4"/>
-        <v>17.392154056914798</v>
-      </c>
-      <c r="AL25" s="42">
-        <f t="shared" si="5"/>
-        <v>14.493461714095666</v>
+      <c r="AH25" s="78">
+        <v>50</v>
+      </c>
+      <c r="AI25" s="72">
+        <f>EXP(LN(0.5)*AH25/10)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="AJ25" s="79">
+        <f>$AJ$15*AI25</f>
+        <v>7.3125</v>
+      </c>
+      <c r="AK25" s="79">
+        <f>$AK$15*AI25</f>
+        <v>4.3875000000000002</v>
+      </c>
+      <c r="AL25" s="79">
+        <f>$AL$15*AI25</f>
+        <v>2.6324999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="L26" s="14"/>
-      <c r="AI26" s="50"/>
-      <c r="AJ26" s="51"/>
-      <c r="AK26" s="51"/>
-      <c r="AL26" s="51"/>
+      <c r="AG26" s="72"/>
+      <c r="AH26" s="78"/>
+      <c r="AI26" s="72"/>
+      <c r="AJ26" s="80"/>
+      <c r="AK26" s="80"/>
+      <c r="AL26" s="80"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI27" s="50"/>
-      <c r="AJ27" s="51"/>
-      <c r="AK27" s="51"/>
-      <c r="AL27" s="51"/>
+    <row r="27" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AG27" s="72"/>
+      <c r="AH27" s="78"/>
+      <c r="AI27" s="72"/>
+      <c r="AJ27" s="81"/>
+      <c r="AK27" s="81"/>
+      <c r="AL27" s="81"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AG30" s="49" t="s">
+    <row r="28" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AG28" s="72"/>
+      <c r="AH28" s="78"/>
+      <c r="AI28" s="72"/>
+      <c r="AJ28" s="72"/>
+      <c r="AK28" s="72"/>
+      <c r="AL28" s="72"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="AG29" s="72"/>
+      <c r="AH29" s="72"/>
+      <c r="AI29" s="72"/>
+      <c r="AJ29" s="72"/>
+      <c r="AK29" s="72"/>
+      <c r="AL29" s="72"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="AG30" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="AJ30" s="74" t="s">
+      <c r="AH30" s="72"/>
+      <c r="AI30" s="72"/>
+      <c r="AJ30" s="75" t="s">
         <v>106</v>
       </c>
-      <c r="AK30" s="74"/>
-      <c r="AL30" s="74"/>
+      <c r="AK30" s="75"/>
+      <c r="AL30" s="75"/>
     </row>
-    <row r="31" spans="1:38" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="59" t="s">
+    <row r="31" spans="1:38" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="53" t="s">
         <v>107</v>
       </c>
       <c r="B31">
@@ -15320,23 +15372,24 @@
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
       <c r="AF31" s="30"/>
-      <c r="AG31" s="49" t="s">
+      <c r="AG31" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="AI31" s="18" t="s">
+      <c r="AH31" s="72"/>
+      <c r="AI31" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="AJ31" s="18" t="s">
+      <c r="AJ31" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="AK31" s="18" t="s">
+      <c r="AK31" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="AL31" s="18" t="s">
+      <c r="AL31" s="74" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O32" s="32"/>
       <c r="P32" s="32"/>
       <c r="Q32" s="32"/>
@@ -15354,20 +15407,22 @@
       <c r="AC32" s="32"/>
       <c r="AD32" s="32"/>
       <c r="AE32" s="32"/>
-      <c r="AG32" s="48" t="s">
+      <c r="AG32" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="AJ32" s="43">
+      <c r="AH32" s="72"/>
+      <c r="AI32" s="72"/>
+      <c r="AJ32" s="77">
         <v>0</v>
       </c>
-      <c r="AK32" s="43">
+      <c r="AK32" s="77">
         <v>0</v>
       </c>
-      <c r="AL32" s="43">
+      <c r="AL32" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O33" s="33"/>
       <c r="P33" s="34">
         <v>1990</v>
@@ -15417,91 +15472,94 @@
       <c r="AE33" s="34">
         <v>2005</v>
       </c>
-      <c r="AG33" s="48" t="s">
+      <c r="AG33" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="AJ33" s="43">
+      <c r="AH33" s="72"/>
+      <c r="AI33" s="72"/>
+      <c r="AJ33" s="77">
         <v>0</v>
       </c>
-      <c r="AK33" s="43">
+      <c r="AK33" s="77">
         <v>0</v>
       </c>
-      <c r="AL33" s="43">
+      <c r="AL33" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O34" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="P34" s="63">
+      <c r="P34" s="57">
         <v>0</v>
       </c>
-      <c r="Q34" s="63">
+      <c r="Q34" s="57">
         <v>0</v>
       </c>
-      <c r="R34" s="63">
+      <c r="R34" s="57">
         <v>0</v>
       </c>
-      <c r="S34" s="63">
+      <c r="S34" s="57">
         <v>0</v>
       </c>
-      <c r="T34" s="63">
+      <c r="T34" s="57">
         <v>0</v>
       </c>
-      <c r="U34" s="63">
+      <c r="U34" s="57">
         <v>0</v>
       </c>
-      <c r="V34" s="63">
+      <c r="V34" s="57">
         <v>0</v>
       </c>
-      <c r="W34" s="63">
+      <c r="W34" s="57">
         <v>0</v>
       </c>
-      <c r="X34" s="63">
+      <c r="X34" s="57">
         <v>0</v>
       </c>
-      <c r="Y34" s="63">
+      <c r="Y34" s="57">
         <v>0</v>
       </c>
-      <c r="Z34" s="63">
+      <c r="Z34" s="57">
         <v>0</v>
       </c>
-      <c r="AA34" s="63">
+      <c r="AA34" s="57">
         <v>0</v>
       </c>
-      <c r="AB34" s="63">
+      <c r="AB34" s="57">
         <v>0</v>
       </c>
-      <c r="AC34" s="63">
+      <c r="AC34" s="57">
         <v>0</v>
       </c>
-      <c r="AD34" s="63">
+      <c r="AD34" s="57">
         <v>0</v>
       </c>
-      <c r="AE34" s="63">
+      <c r="AE34" s="57">
         <v>0</v>
       </c>
-      <c r="AG34" s="48" t="s">
+      <c r="AG34" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="AI34">
-        <v>0.27</v>
-      </c>
-      <c r="AJ34" s="43">
+      <c r="AH34" s="72"/>
+      <c r="AI34" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="AJ34" s="77">
         <f>AI34*$AJ$36</f>
-        <v>63.180000000000007</v>
-      </c>
-      <c r="AK34" s="43">
+        <v>11.700000000000001</v>
+      </c>
+      <c r="AK34" s="77">
         <f>AK36*AI34</f>
-        <v>31.590000000000003</v>
-      </c>
-      <c r="AL34" s="43">
+        <v>7.0200000000000005</v>
+      </c>
+      <c r="AL34" s="77">
         <f>AL36*AI34</f>
-        <v>26.325000000000003</v>
+        <v>4.2119999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -15514,74 +15572,75 @@
       <c r="O35" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="P35" s="63">
+      <c r="P35" s="57">
         <v>0</v>
       </c>
-      <c r="Q35" s="63">
+      <c r="Q35" s="57">
         <v>0</v>
       </c>
-      <c r="R35" s="63">
+      <c r="R35" s="57">
         <v>0</v>
       </c>
-      <c r="S35" s="63">
+      <c r="S35" s="57">
         <v>0</v>
       </c>
-      <c r="T35" s="63">
+      <c r="T35" s="57">
         <v>0</v>
       </c>
-      <c r="U35" s="63">
+      <c r="U35" s="57">
         <v>0</v>
       </c>
-      <c r="V35" s="63">
+      <c r="V35" s="57">
         <v>0</v>
       </c>
-      <c r="W35" s="63">
+      <c r="W35" s="57">
         <v>0</v>
       </c>
-      <c r="X35" s="63">
+      <c r="X35" s="57">
         <v>0</v>
       </c>
-      <c r="Y35" s="63">
+      <c r="Y35" s="57">
         <v>0</v>
       </c>
-      <c r="Z35" s="63">
+      <c r="Z35" s="57">
         <v>0</v>
       </c>
-      <c r="AA35" s="63">
+      <c r="AA35" s="57">
         <v>0</v>
       </c>
-      <c r="AB35" s="63">
+      <c r="AB35" s="57">
         <v>0</v>
       </c>
-      <c r="AC35" s="63">
+      <c r="AC35" s="57">
         <v>0</v>
       </c>
-      <c r="AD35" s="63">
+      <c r="AD35" s="57">
         <v>0</v>
       </c>
-      <c r="AE35" s="63">
+      <c r="AE35" s="57">
         <v>0</v>
       </c>
-      <c r="AG35" s="48" t="s">
+      <c r="AG35" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="AI35">
-        <v>0.9</v>
-      </c>
-      <c r="AJ35" s="43">
+      <c r="AH35" s="72"/>
+      <c r="AI35" s="72">
+        <v>0.7</v>
+      </c>
+      <c r="AJ35" s="77">
         <f>AI35*$AJ$36</f>
-        <v>210.6</v>
-      </c>
-      <c r="AK35" s="43">
+        <v>163.79999999999998</v>
+      </c>
+      <c r="AK35" s="77">
         <f>AI35*AK36</f>
-        <v>105.3</v>
-      </c>
-      <c r="AL35" s="43">
+        <v>98.28</v>
+      </c>
+      <c r="AL35" s="77">
         <f>AL36*AI35</f>
-        <v>87.75</v>
+        <v>58.967999999999989</v>
       </c>
     </row>
-    <row r="36" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>15</v>
       </c>
@@ -15595,78 +15654,72 @@
       <c r="O36" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="P36" s="63">
+      <c r="P36" s="57">
         <v>0</v>
       </c>
-      <c r="Q36" s="63">
+      <c r="Q36" s="57">
         <v>0</v>
       </c>
-      <c r="R36" s="63">
+      <c r="R36" s="57">
         <v>0</v>
       </c>
-      <c r="S36" s="63">
+      <c r="S36" s="57">
         <v>0</v>
       </c>
-      <c r="T36" s="63">
+      <c r="T36" s="57">
         <v>0</v>
       </c>
-      <c r="U36" s="63">
+      <c r="U36" s="57">
         <v>0</v>
       </c>
-      <c r="V36" s="63">
+      <c r="V36" s="57">
         <v>0</v>
       </c>
-      <c r="W36" s="63">
+      <c r="W36" s="57">
         <v>0</v>
       </c>
-      <c r="X36" s="63">
+      <c r="X36" s="57">
         <v>0</v>
       </c>
-      <c r="Y36" s="63">
+      <c r="Y36" s="57">
         <v>0</v>
       </c>
-      <c r="Z36" s="63">
+      <c r="Z36" s="57">
         <v>0</v>
       </c>
-      <c r="AA36" s="63">
+      <c r="AA36" s="57">
         <v>0</v>
       </c>
-      <c r="AB36" s="63">
+      <c r="AB36" s="57">
         <v>0</v>
       </c>
-      <c r="AC36" s="63">
+      <c r="AC36" s="57">
         <v>0</v>
       </c>
-      <c r="AD36" s="63">
+      <c r="AD36" s="57">
         <v>0</v>
       </c>
-      <c r="AE36" s="63">
+      <c r="AE36" s="57">
         <v>0</v>
       </c>
-      <c r="AG36" s="48" t="s">
+      <c r="AG36" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="AH36" s="12">
+      <c r="AH36" s="78">
         <v>1</v>
       </c>
-      <c r="AI36">
-        <f>EXP(LN(0.5)*AH36/20)</f>
-        <v>0.9659363289248456</v>
-      </c>
-      <c r="AJ36" s="43">
-        <f>AI3</f>
+      <c r="AI36" s="72"/>
+      <c r="AJ36" s="77">
         <v>234</v>
       </c>
-      <c r="AK36" s="43">
-        <f>AJ3</f>
-        <v>117</v>
-      </c>
-      <c r="AL36" s="43">
-        <f>AK3</f>
-        <v>97.5</v>
+      <c r="AK36" s="77">
+        <v>140.4</v>
+      </c>
+      <c r="AL36" s="77">
+        <v>84.24</v>
       </c>
     </row>
-    <row r="37" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="6" t="s">
         <v>22</v>
       </c>
@@ -15679,78 +15732,77 @@
       <c r="O37" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="P37" s="64">
+      <c r="P37" s="58">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="Q37" s="64">
+      <c r="Q37" s="58">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="R37" s="64">
+      <c r="R37" s="58">
         <v>0.10100000000000001</v>
       </c>
-      <c r="S37" s="64">
+      <c r="S37" s="58">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="T37" s="64">
+      <c r="T37" s="58">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="U37" s="64">
+      <c r="U37" s="58">
         <v>0.10199999999999999</v>
       </c>
-      <c r="V37" s="64">
+      <c r="V37" s="58">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="W37" s="64">
+      <c r="W37" s="58">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="X37" s="64">
+      <c r="X37" s="58">
         <v>0.09</v>
       </c>
-      <c r="Y37" s="64">
+      <c r="Y37" s="58">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="Z37" s="64">
+      <c r="Z37" s="58">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="AA37" s="64">
+      <c r="AA37" s="58">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="AB37" s="64">
+      <c r="AB37" s="58">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="AC37" s="64">
+      <c r="AC37" s="58">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="AD37" s="64">
+      <c r="AD37" s="58">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AE37" s="64">
+      <c r="AE37" s="58">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="AG37" s="48" t="s">
+      <c r="AG37" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="AH37" s="12">
+      <c r="AH37" s="78">
         <v>5</v>
       </c>
-      <c r="AI37">
-        <f t="shared" ref="AI37:AI43" si="6">EXP(LN(0.5)*AH37/20)</f>
-        <v>0.8408964152537145</v>
-      </c>
-      <c r="AJ37" s="43">
-        <f t="shared" ref="AJ37:AJ47" si="7">$AJ$36*AI37</f>
-        <v>196.76976116936919</v>
-      </c>
-      <c r="AK37" s="43">
-        <f t="shared" ref="AK37:AK47" si="8">$AK$36*AI37</f>
-        <v>98.384880584684595</v>
-      </c>
-      <c r="AL37" s="43">
-        <f>$AK$3*AI37</f>
-        <v>81.987400487237167</v>
+      <c r="AI37" s="72">
+        <f>EXP(LN(0.5)*AH37/10)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="AJ37" s="77">
+        <f>$AJ$36*AI37</f>
+        <v>165.46298679765212</v>
+      </c>
+      <c r="AK37" s="77">
+        <f>$AK$36*AI37</f>
+        <v>99.27779207859129</v>
+      </c>
+      <c r="AL37" s="77">
+        <v>59.566675247154762</v>
       </c>
     </row>
-    <row r="38" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="6" t="s">
         <v>25</v>
       </c>
@@ -15763,78 +15815,77 @@
       <c r="O38" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="P38" s="64">
+      <c r="P38" s="58">
         <v>0.191</v>
       </c>
-      <c r="Q38" s="64">
+      <c r="Q38" s="58">
         <v>0.19</v>
       </c>
-      <c r="R38" s="64">
+      <c r="R38" s="58">
         <v>0.186</v>
       </c>
-      <c r="S38" s="64">
+      <c r="S38" s="58">
         <v>0.17599999999999999</v>
       </c>
-      <c r="T38" s="64">
+      <c r="T38" s="58">
         <v>0.158</v>
       </c>
-      <c r="U38" s="64">
+      <c r="U38" s="58">
         <v>0.14299999999999999</v>
       </c>
-      <c r="V38" s="64">
+      <c r="V38" s="58">
         <v>0.14699999999999999</v>
       </c>
-      <c r="W38" s="64">
+      <c r="W38" s="58">
         <v>0.16600000000000001</v>
       </c>
-      <c r="X38" s="64">
+      <c r="X38" s="58">
         <v>0.14199999999999999</v>
       </c>
-      <c r="Y38" s="64">
+      <c r="Y38" s="58">
         <v>0.154</v>
       </c>
-      <c r="Z38" s="64">
+      <c r="Z38" s="58">
         <v>0.13700000000000001</v>
       </c>
-      <c r="AA38" s="64">
+      <c r="AA38" s="58">
         <v>0.13400000000000001</v>
       </c>
-      <c r="AB38" s="64">
+      <c r="AB38" s="58">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AC38" s="64">
+      <c r="AC38" s="58">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AD38" s="64">
+      <c r="AD38" s="58">
         <v>0.14699999999999999</v>
       </c>
-      <c r="AE38" s="64">
+      <c r="AE38" s="58">
         <v>0.152</v>
       </c>
-      <c r="AG38" s="48" t="s">
+      <c r="AG38" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="AH38" s="12">
+      <c r="AH38" s="78">
         <v>10</v>
       </c>
-      <c r="AI38">
-        <f t="shared" si="6"/>
-        <v>0.70710678118654757</v>
-      </c>
-      <c r="AJ38" s="43">
-        <f t="shared" si="7"/>
-        <v>165.46298679765212</v>
-      </c>
-      <c r="AK38" s="43">
-        <f t="shared" si="8"/>
-        <v>82.731493398826061</v>
-      </c>
-      <c r="AL38" s="43">
-        <f t="shared" ref="AL38:AL43" si="9">$AK$3*AI38</f>
-        <v>68.942911165688386</v>
+      <c r="AI38" s="72">
+        <f>EXP(LN(0.5)*AH38/10)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AJ38" s="77">
+        <f>$AJ$36*AI38</f>
+        <v>117</v>
+      </c>
+      <c r="AK38" s="77">
+        <f>$AK$36*AI38</f>
+        <v>70.2</v>
+      </c>
+      <c r="AL38" s="77">
+        <v>42.12</v>
       </c>
     </row>
-    <row r="39" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>28</v>
       </c>
@@ -15847,78 +15898,77 @@
       <c r="O39" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="P39" s="64">
+      <c r="P39" s="58">
         <v>0.19700000000000001</v>
       </c>
-      <c r="Q39" s="64">
+      <c r="Q39" s="58">
         <v>0.20499999999999999</v>
       </c>
-      <c r="R39" s="64">
+      <c r="R39" s="58">
         <v>0.20100000000000001</v>
       </c>
-      <c r="S39" s="64">
+      <c r="S39" s="58">
         <v>0.185</v>
       </c>
-      <c r="T39" s="64">
+      <c r="T39" s="58">
         <v>0.184</v>
       </c>
-      <c r="U39" s="64">
+      <c r="U39" s="58">
         <v>0.17899999999999999</v>
       </c>
-      <c r="V39" s="64">
+      <c r="V39" s="58">
         <v>0.161</v>
       </c>
-      <c r="W39" s="64">
+      <c r="W39" s="58">
         <v>0.17199999999999999</v>
       </c>
-      <c r="X39" s="64">
+      <c r="X39" s="58">
         <v>0.13300000000000001</v>
       </c>
-      <c r="Y39" s="64">
+      <c r="Y39" s="58">
         <v>0.14399999999999999</v>
       </c>
-      <c r="Z39" s="64">
+      <c r="Z39" s="58">
         <v>0.13300000000000001</v>
       </c>
-      <c r="AA39" s="64">
+      <c r="AA39" s="58">
         <v>0.13</v>
       </c>
-      <c r="AB39" s="64">
+      <c r="AB39" s="58">
         <v>0.13500000000000001</v>
       </c>
-      <c r="AC39" s="64">
+      <c r="AC39" s="58">
         <v>0.13100000000000001</v>
       </c>
-      <c r="AD39" s="64">
+      <c r="AD39" s="58">
         <v>0.126</v>
       </c>
-      <c r="AE39" s="64">
+      <c r="AE39" s="58">
         <v>0.11700000000000001</v>
       </c>
-      <c r="AG39" s="48" t="s">
+      <c r="AG39" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="AH39" s="12">
+      <c r="AH39" s="78">
         <v>15</v>
       </c>
-      <c r="AI39">
-        <f t="shared" si="6"/>
-        <v>0.59460355750136051</v>
-      </c>
-      <c r="AJ39" s="43">
-        <f t="shared" si="7"/>
-        <v>139.13723245531835</v>
-      </c>
-      <c r="AK39" s="43">
-        <f t="shared" si="8"/>
-        <v>69.568616227659177</v>
-      </c>
-      <c r="AL39" s="43">
-        <f t="shared" si="9"/>
-        <v>57.97384685638265</v>
+      <c r="AI39" s="72">
+        <f>EXP(LN(0.5)*AH39/10)</f>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="AJ39" s="77">
+        <f>$AJ$36*AI39*0.7</f>
+        <v>57.912045379178238</v>
+      </c>
+      <c r="AK39" s="77">
+        <f>$AK$36*AI39*0.7</f>
+        <v>34.747227227506947</v>
+      </c>
+      <c r="AL39" s="77">
+        <v>20.848336336504165</v>
       </c>
     </row>
-    <row r="40" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="6" t="s">
         <v>30</v>
       </c>
@@ -15931,78 +15981,77 @@
       <c r="O40" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="P40" s="64">
+      <c r="P40" s="58">
         <v>0.219</v>
       </c>
-      <c r="Q40" s="64">
+      <c r="Q40" s="58">
         <v>0.192</v>
       </c>
-      <c r="R40" s="64">
+      <c r="R40" s="58">
         <v>0.17499999999999999</v>
       </c>
-      <c r="S40" s="64">
+      <c r="S40" s="58">
         <v>0.18099999999999999</v>
       </c>
-      <c r="T40" s="64">
+      <c r="T40" s="58">
         <v>0.17199999999999999</v>
       </c>
-      <c r="U40" s="64">
+      <c r="U40" s="58">
         <v>0.16400000000000001</v>
       </c>
-      <c r="V40" s="64">
+      <c r="V40" s="58">
         <v>0.161</v>
       </c>
-      <c r="W40" s="64">
+      <c r="W40" s="58">
         <v>0.159</v>
       </c>
-      <c r="X40" s="64">
+      <c r="X40" s="58">
         <v>0.13900000000000001</v>
       </c>
-      <c r="Y40" s="64">
+      <c r="Y40" s="58">
         <v>0.14499999999999999</v>
       </c>
-      <c r="Z40" s="64">
+      <c r="Z40" s="58">
         <v>0.12</v>
       </c>
-      <c r="AA40" s="64">
+      <c r="AA40" s="58">
         <v>0.12</v>
       </c>
-      <c r="AB40" s="64">
+      <c r="AB40" s="58">
         <v>0.105</v>
       </c>
-      <c r="AC40" s="64">
+      <c r="AC40" s="58">
         <v>0.125</v>
       </c>
-      <c r="AD40" s="64">
+      <c r="AD40" s="58">
         <v>0.108</v>
       </c>
-      <c r="AE40" s="64">
+      <c r="AE40" s="58">
         <v>0.10199999999999999</v>
       </c>
-      <c r="AG40" s="48" t="s">
+      <c r="AG40" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="AH40" s="12">
+      <c r="AH40" s="78">
         <v>20</v>
       </c>
-      <c r="AI40">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="AJ40" s="43">
-        <f t="shared" si="7"/>
-        <v>117</v>
-      </c>
-      <c r="AK40" s="43">
-        <f t="shared" si="8"/>
-        <v>58.5</v>
-      </c>
-      <c r="AL40" s="43">
-        <f t="shared" si="9"/>
-        <v>48.75</v>
+      <c r="AI40" s="72">
+        <f>EXP(LN(0.5)*AH40/10)</f>
+        <v>0.25</v>
+      </c>
+      <c r="AJ40" s="77">
+        <f>$AJ$36*AI40*0.7</f>
+        <v>40.949999999999996</v>
+      </c>
+      <c r="AK40" s="77">
+        <f>$AK$36*AI40*0.7</f>
+        <v>24.57</v>
+      </c>
+      <c r="AL40" s="77">
+        <v>14.741999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="6" t="s">
         <v>31</v>
       </c>
@@ -16015,78 +16064,77 @@
       <c r="O41" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="P41" s="64">
+      <c r="P41" s="58">
         <v>0.13400000000000001</v>
       </c>
-      <c r="Q41" s="64">
+      <c r="Q41" s="58">
         <v>0.13200000000000001</v>
       </c>
-      <c r="R41" s="64">
+      <c r="R41" s="58">
         <v>0.13700000000000001</v>
       </c>
-      <c r="S41" s="64">
+      <c r="S41" s="58">
         <v>0.127</v>
       </c>
-      <c r="T41" s="64">
+      <c r="T41" s="58">
         <v>0.114</v>
       </c>
-      <c r="U41" s="64">
+      <c r="U41" s="58">
         <v>0.1</v>
       </c>
-      <c r="V41" s="64">
+      <c r="V41" s="58">
         <v>0.112</v>
       </c>
-      <c r="W41" s="64">
+      <c r="W41" s="58">
         <v>0.115</v>
       </c>
-      <c r="X41" s="64">
+      <c r="X41" s="58">
         <v>0.105</v>
       </c>
-      <c r="Y41" s="64">
+      <c r="Y41" s="58">
         <v>0.09</v>
       </c>
-      <c r="Z41" s="64">
+      <c r="Z41" s="58">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="AA41" s="64">
+      <c r="AA41" s="58">
         <v>0.09</v>
       </c>
-      <c r="AB41" s="64">
+      <c r="AB41" s="58">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="AC41" s="64">
+      <c r="AC41" s="58">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="AD41" s="64">
+      <c r="AD41" s="58">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="AE41" s="64">
+      <c r="AE41" s="58">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="AG41" s="48" t="s">
+      <c r="AG41" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="AH41" s="12">
+      <c r="AH41" s="78">
         <v>25</v>
       </c>
-      <c r="AI41">
-        <f t="shared" si="6"/>
-        <v>0.42044820762685725</v>
-      </c>
-      <c r="AJ41" s="43">
-        <f t="shared" si="7"/>
-        <v>98.384880584684595</v>
-      </c>
-      <c r="AK41" s="43">
-        <f t="shared" si="8"/>
-        <v>49.192440292342297</v>
-      </c>
-      <c r="AL41" s="43">
-        <f t="shared" si="9"/>
-        <v>40.993700243618584</v>
+      <c r="AI41" s="72">
+        <f>EXP(LN(0.5)*AH41/10)</f>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="AJ41" s="77">
+        <f>$AJ$36*AI41*0.5</f>
+        <v>20.682873349706515</v>
+      </c>
+      <c r="AK41" s="77">
+        <f>$AK$36*AI41*0.5</f>
+        <v>12.409724009823911</v>
+      </c>
+      <c r="AL41" s="77">
+        <v>7.4458344058943453</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
@@ -16099,78 +16147,77 @@
       <c r="O42" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="P42" s="64">
+      <c r="P42" s="58">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="Q42" s="64">
+      <c r="Q42" s="58">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="R42" s="64">
+      <c r="R42" s="58">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="S42" s="64">
+      <c r="S42" s="58">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="T42" s="64">
+      <c r="T42" s="58">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="U42" s="64">
+      <c r="U42" s="58">
         <v>0.05</v>
       </c>
-      <c r="V42" s="64">
+      <c r="V42" s="58">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="W42" s="64">
+      <c r="W42" s="58">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="X42" s="64">
+      <c r="X42" s="58">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="Y42" s="64">
+      <c r="Y42" s="58">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="Z42" s="64">
+      <c r="Z42" s="58">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="AA42" s="64">
+      <c r="AA42" s="58">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AB42" s="64">
+      <c r="AB42" s="58">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AC42" s="64">
+      <c r="AC42" s="58">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AD42" s="64">
+      <c r="AD42" s="58">
         <v>3.1E-2</v>
       </c>
-      <c r="AE42" s="64">
+      <c r="AE42" s="58">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="AG42" s="48" t="s">
+      <c r="AG42" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="AH42" s="12">
+      <c r="AH42" s="78">
         <v>30</v>
       </c>
-      <c r="AI42">
-        <f t="shared" si="6"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="AJ42" s="43">
-        <f t="shared" si="7"/>
-        <v>82.731493398826061</v>
-      </c>
-      <c r="AK42" s="43">
-        <f t="shared" si="8"/>
-        <v>41.36574669941303</v>
-      </c>
-      <c r="AL42" s="43">
-        <f t="shared" si="9"/>
-        <v>34.471455582844193</v>
+      <c r="AI42" s="72">
+        <f>EXP(LN(0.5)*AH42/10)</f>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="AJ42" s="77">
+        <f>$AJ$36*AI42</f>
+        <v>29.250000000000007</v>
+      </c>
+      <c r="AK42" s="77">
+        <f>$AK$36*AI42</f>
+        <v>17.550000000000004</v>
+      </c>
+      <c r="AL42" s="77">
+        <v>10.530000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="6" t="s">
         <v>33</v>
       </c>
@@ -16183,78 +16230,77 @@
       <c r="O43" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="P43" s="64">
+      <c r="P43" s="58">
         <v>0.01</v>
       </c>
-      <c r="Q43" s="64">
+      <c r="Q43" s="58">
         <v>0.01</v>
       </c>
-      <c r="R43" s="64">
+      <c r="R43" s="58">
         <v>0.01</v>
       </c>
-      <c r="S43" s="64">
+      <c r="S43" s="58">
         <v>0.01</v>
       </c>
-      <c r="T43" s="64">
+      <c r="T43" s="58">
         <v>0.01</v>
       </c>
-      <c r="U43" s="64">
+      <c r="U43" s="58">
         <v>0.01</v>
       </c>
-      <c r="V43" s="64">
+      <c r="V43" s="58">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="W43" s="64">
+      <c r="W43" s="58">
         <v>0.01</v>
       </c>
-      <c r="X43" s="64">
+      <c r="X43" s="58">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="Y43" s="64">
+      <c r="Y43" s="58">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="Z43" s="64">
+      <c r="Z43" s="58">
         <v>1.2E-2</v>
       </c>
-      <c r="AA43" s="64">
+      <c r="AA43" s="58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AB43" s="64">
+      <c r="AB43" s="58">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AC43" s="64">
+      <c r="AC43" s="58">
         <v>2E-3</v>
       </c>
-      <c r="AD43" s="64">
+      <c r="AD43" s="58">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AE43" s="64">
+      <c r="AE43" s="58">
         <v>2E-3</v>
       </c>
-      <c r="AG43" s="48" t="s">
+      <c r="AG43" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="AH43" s="12">
+      <c r="AH43" s="78">
         <v>35</v>
       </c>
-      <c r="AI43">
-        <f t="shared" si="6"/>
-        <v>0.29730177875068031</v>
-      </c>
-      <c r="AJ43" s="43">
-        <f t="shared" si="7"/>
-        <v>69.568616227659192</v>
-      </c>
-      <c r="AK43" s="43">
-        <f t="shared" si="8"/>
-        <v>34.784308113829596</v>
-      </c>
-      <c r="AL43" s="43">
-        <f t="shared" si="9"/>
-        <v>28.986923428191332</v>
+      <c r="AI43" s="72">
+        <f>EXP(LN(0.5)*AH43/10)</f>
+        <v>8.8388347648318447E-2</v>
+      </c>
+      <c r="AJ43" s="77">
+        <f>$AJ$36*AI43</f>
+        <v>20.682873349706515</v>
+      </c>
+      <c r="AK43" s="77">
+        <f>$AK$36*AI43</f>
+        <v>12.409724009823911</v>
+      </c>
+      <c r="AL43" s="77">
+        <v>7.4458344058943453</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="6" t="s">
         <v>35</v>
       </c>
@@ -16267,78 +16313,77 @@
       <c r="O44" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="P44" s="65">
+      <c r="P44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="Q44" s="65">
+      <c r="Q44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="R44" s="65">
+      <c r="R44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="S44" s="65">
+      <c r="S44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="T44" s="65">
+      <c r="T44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="U44" s="65">
+      <c r="U44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="V44" s="65">
+      <c r="V44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="W44" s="65">
+      <c r="W44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="X44" s="65">
+      <c r="X44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="Y44" s="65">
+      <c r="Y44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="Z44" s="65">
+      <c r="Z44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="AA44" s="65">
+      <c r="AA44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="AB44" s="65">
+      <c r="AB44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="AC44" s="65">
+      <c r="AC44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="AD44" s="65">
+      <c r="AD44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="AE44" s="65">
+      <c r="AE44" s="59">
         <v>1.711E-2</v>
       </c>
-      <c r="AG44" s="48" t="s">
+      <c r="AG44" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="AH44" s="12">
+      <c r="AH44" s="78">
         <v>40</v>
       </c>
-      <c r="AI44">
-        <f t="shared" ref="AI44:AI47" si="10">EXP(LN(0.5)*AH44/20)</f>
-        <v>0.25</v>
-      </c>
-      <c r="AJ44" s="43">
-        <f t="shared" si="7"/>
-        <v>58.5</v>
-      </c>
-      <c r="AK44" s="43">
-        <f t="shared" si="8"/>
-        <v>29.25</v>
-      </c>
-      <c r="AL44" s="43">
-        <f t="shared" ref="AL44:AL47" si="11">$AK$3*AI44</f>
-        <v>24.375</v>
+      <c r="AI44" s="72">
+        <f>EXP(LN(0.5)*AH44/10)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AJ44" s="77">
+        <f>$AJ$36*AI44</f>
+        <v>14.625</v>
+      </c>
+      <c r="AK44" s="77">
+        <f>$AK$36*AI44</f>
+        <v>8.7750000000000004</v>
+      </c>
+      <c r="AL44" s="77">
+        <v>5.2649999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
@@ -16351,78 +16396,77 @@
       <c r="O45" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="P45" s="65">
+      <c r="P45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Q45" s="65">
+      <c r="Q45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="R45" s="65">
+      <c r="R45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="S45" s="65">
+      <c r="S45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="T45" s="65">
+      <c r="T45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="U45" s="65">
+      <c r="U45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="V45" s="65">
+      <c r="V45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="W45" s="65">
+      <c r="W45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="X45" s="65">
+      <c r="X45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Y45" s="65">
+      <c r="Y45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="Z45" s="65">
+      <c r="Z45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="AA45" s="65">
+      <c r="AA45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="AB45" s="65">
+      <c r="AB45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="AC45" s="65">
+      <c r="AC45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="AD45" s="65">
+      <c r="AD45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="AE45" s="65">
+      <c r="AE45" s="59">
         <v>2.0809999999999999E-2</v>
       </c>
-      <c r="AG45" s="48" t="s">
+      <c r="AG45" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="AH45" s="12">
+      <c r="AH45" s="78">
         <v>45</v>
       </c>
-      <c r="AI45">
-        <f t="shared" si="10"/>
-        <v>0.21022410381342865</v>
-      </c>
-      <c r="AJ45" s="43">
-        <f t="shared" si="7"/>
-        <v>49.192440292342305</v>
-      </c>
-      <c r="AK45" s="43">
-        <f t="shared" si="8"/>
-        <v>24.596220146171152</v>
-      </c>
-      <c r="AL45" s="43">
-        <f t="shared" si="11"/>
-        <v>20.496850121809295</v>
+      <c r="AI45" s="72">
+        <f>EXP(LN(0.5)*AH45/10)</f>
+        <v>4.4194173824159223E-2</v>
+      </c>
+      <c r="AJ45" s="77">
+        <f>$AJ$36*AI45</f>
+        <v>10.341436674853258</v>
+      </c>
+      <c r="AK45" s="77">
+        <f>$AK$36*AI45</f>
+        <v>6.2048620049119556</v>
+      </c>
+      <c r="AL45" s="77">
+        <v>3.7229172029471727</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="6" t="s">
         <v>37</v>
       </c>
@@ -16483,37 +16527,36 @@
       <c r="AE46" s="34">
         <v>2.8</v>
       </c>
-      <c r="AG46" s="48" t="s">
+      <c r="AG46" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="AH46" s="12">
+      <c r="AH46" s="78">
         <v>50</v>
       </c>
-      <c r="AI46">
-        <f t="shared" si="10"/>
-        <v>0.17677669529663689</v>
-      </c>
-      <c r="AJ46" s="43">
-        <f t="shared" si="7"/>
-        <v>41.36574669941303</v>
-      </c>
-      <c r="AK46" s="43">
-        <f t="shared" si="8"/>
-        <v>20.682873349706515</v>
-      </c>
-      <c r="AL46" s="43">
-        <f t="shared" si="11"/>
-        <v>17.235727791422097</v>
+      <c r="AI46" s="72">
+        <f>EXP(LN(0.5)*AH46/10)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="AJ46" s="77">
+        <f>$AJ$36*AI46</f>
+        <v>7.3125</v>
+      </c>
+      <c r="AK46" s="77">
+        <f>$AK$36*AI46</f>
+        <v>4.3875000000000002</v>
+      </c>
+      <c r="AL46" s="77">
+        <v>2.6324999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="55" t="s">
+    <row r="47" spans="1:38" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="56">
+      <c r="B47" s="50">
         <v>-70487</v>
       </c>
-      <c r="C47" s="56">
+      <c r="C47" s="50">
         <v>82330</v>
       </c>
       <c r="P47" s="30"/>
@@ -16527,37 +16570,36 @@
       <c r="X47" s="31"/>
       <c r="Y47" s="31"/>
       <c r="Z47" s="30"/>
-      <c r="AG47" s="48" t="s">
+      <c r="AG47" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="AH47" s="12">
+      <c r="AH47" s="78">
         <v>55</v>
       </c>
-      <c r="AI47">
-        <f t="shared" si="10"/>
-        <v>0.14865088937534016</v>
-      </c>
-      <c r="AJ47" s="43">
-        <f t="shared" si="7"/>
-        <v>34.784308113829596</v>
-      </c>
-      <c r="AK47" s="43">
-        <f t="shared" si="8"/>
-        <v>17.392154056914798</v>
-      </c>
-      <c r="AL47" s="43">
-        <f t="shared" si="11"/>
-        <v>14.493461714095666</v>
+      <c r="AI47" s="72">
+        <f>EXP(LN(0.5)*AH47/10)</f>
+        <v>2.2097086912079619E-2</v>
+      </c>
+      <c r="AJ47" s="77">
+        <f>$AJ$36*AI47</f>
+        <v>5.1707183374266306</v>
+      </c>
+      <c r="AK47" s="77">
+        <f>$AK$36*AI47</f>
+        <v>3.1024310024559787</v>
+      </c>
+      <c r="AL47" s="77">
+        <v>1.861458601473587</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="53" t="s">
+    <row r="48" spans="1:38" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="57">
+      <c r="B48" s="51">
         <v>-50094.736842105267</v>
       </c>
-      <c r="C48" s="57">
+      <c r="C48" s="51">
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
@@ -16565,26 +16607,26 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A49" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="57">
+      <c r="B49" s="51">
         <v>-35803.827751196171</v>
       </c>
-      <c r="C49" s="57">
+      <c r="C49" s="51">
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="53" t="s">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A50" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="57">
+      <c r="B50" s="51">
         <v>-24102.551834130783</v>
       </c>
-      <c r="C50" s="57">
+      <c r="C50" s="51">
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
@@ -16592,27 +16634,27 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="53" t="s">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A51" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="57">
+      <c r="B51" s="51">
         <v>-14240.510366826158</v>
       </c>
-      <c r="C51" s="57">
+      <c r="C51" s="51">
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O53" s="29"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="O62" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="O63" t="s">
         <v>68</v>
       </c>
@@ -16620,7 +16662,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="O64" t="s">
         <v>0</v>
       </c>
@@ -16631,7 +16673,7 @@
         <v>0.23480000000000001</v>
       </c>
     </row>
-    <row r="65" spans="15:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O65" t="s">
         <v>1</v>
       </c>
@@ -16642,7 +16684,7 @@
         <v>0.21460000000000001</v>
       </c>
     </row>
-    <row r="69" spans="15:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O69">
         <f>NORMDIST(0.7, P64,Q64,TRUE)</f>
         <v>0.78945004503905036</v>
@@ -16650,18 +16692,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:P3"/>
     <mergeCell ref="AJ8:AL8"/>
     <mergeCell ref="AJ30:AL30"/>
     <mergeCell ref="R1:V1"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16678,22 +16720,22 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="12" max="12" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
-    <col min="15" max="16" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.26953125" customWidth="1"/>
+    <col min="15" max="16" width="11.453125" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="T2" t="s">
         <v>54</v>
       </c>
@@ -16701,23 +16743,23 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
-      <c r="B3" s="78">
+      <c r="B3" s="71">
         <v>1996</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78">
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71">
         <v>2001</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78">
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71">
         <v>2011</v>
       </c>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
       <c r="L3" t="s">
         <v>54</v>
       </c>
@@ -16743,7 +16785,7 @@
         <v>5420315</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -16803,7 +16845,7 @@
         <v>8068284</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>45</v>
       </c>
@@ -16863,7 +16905,7 @@
         <v>9138179</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>46</v>
       </c>
@@ -16923,7 +16965,7 @@
         <v>10267300</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>47</v>
       </c>
@@ -16983,7 +17025,7 @@
         <v>10456909</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -17030,7 +17072,7 @@
         <v>10571313</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="S9" t="s">
         <v>70</v>
       </c>
@@ -17041,7 +17083,7 @@
         <v>10688168</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>51</v>
       </c>
@@ -17095,7 +17137,7 @@
         <v>10806536</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="S11" t="s">
         <v>70</v>
       </c>
@@ -17106,7 +17148,7 @@
         <v>10924776</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -17120,7 +17162,7 @@
         <v>11039740</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>50</v>
       </c>
@@ -17134,7 +17176,7 @@
         <v>11155657</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>52</v>
       </c>
@@ -17143,7 +17185,7 @@
         <v>5.1649773565416463E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -17152,12 +17194,12 @@
         <v>2.0659909426166585E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E32" t="s">
         <v>54</v>
       </c>
@@ -17165,7 +17207,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E33">
         <v>1990</v>
       </c>
@@ -17179,7 +17221,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E34">
         <v>1991</v>
       </c>
@@ -17187,7 +17229,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E35">
         <v>1992</v>
       </c>
@@ -17195,7 +17237,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E36">
         <v>1993</v>
       </c>
@@ -17203,7 +17245,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E37">
         <v>1994</v>
       </c>
@@ -17211,7 +17253,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E38">
         <v>1995</v>
       </c>
@@ -17219,7 +17261,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E39">
         <v>1996</v>
       </c>
@@ -17227,7 +17269,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E40">
         <v>1997</v>
       </c>
@@ -17235,7 +17277,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E41">
         <v>1998</v>
       </c>
@@ -17243,7 +17285,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E42">
         <v>1999</v>
       </c>
@@ -17251,7 +17293,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E43">
         <v>2000</v>
       </c>
@@ -17259,7 +17301,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E44">
         <v>2001</v>
       </c>
@@ -17273,7 +17315,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E45">
         <v>2002</v>
       </c>
@@ -17281,7 +17323,7 @@
         <v>0.24299999999999999</v>
       </c>
     </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E46">
         <v>2003</v>
       </c>
@@ -17289,7 +17331,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E47">
         <v>2004</v>
       </c>
@@ -17297,7 +17339,7 @@
         <v>0.27100000000000002</v>
       </c>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E48">
         <v>2005</v>
       </c>
@@ -17305,7 +17347,7 @@
         <v>0.26100000000000001</v>
       </c>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E49">
         <v>2006</v>
       </c>
@@ -17313,7 +17355,7 @@
         <v>0.26100000000000001</v>
       </c>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E50">
         <v>2007</v>
       </c>
@@ -17321,7 +17363,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E51">
         <v>2008</v>
       </c>
@@ -17329,7 +17371,7 @@
         <v>0.25800000000000001</v>
       </c>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E52">
         <v>2009</v>
       </c>
@@ -17337,7 +17379,7 @@
         <v>0.26300000000000001</v>
       </c>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E53">
         <v>2010</v>
       </c>
@@ -17345,7 +17387,7 @@
         <v>0.26300000000000001</v>
       </c>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E54">
         <v>2012</v>
       </c>
@@ -17356,7 +17398,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:8" x14ac:dyDescent="0.35">
       <c r="F55" s="26"/>
     </row>
   </sheetData>

</xml_diff>